<commit_message>
Create default dispatcher for Code hook and fulfillment.
</commit_message>
<xml_diff>
--- a/playground/MakeAppointmentChatBot.xlsx
+++ b/playground/MakeAppointmentChatBot.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="136">
   <si>
     <t>name</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>sampleUtterances</t>
-  </si>
-  <si>
-    <t>fulfillmentActivity</t>
   </si>
   <si>
     <t>slots</t>
@@ -442,13 +439,7 @@
     <t>AppointmentTypes</t>
   </si>
   <si>
-    <t>dialogCodeHook</t>
-  </si>
-  <si>
     <t>Intent to make appointment</t>
-  </si>
-  <si>
-    <t>appointment</t>
   </si>
 </sst>
 </file>
@@ -801,23 +792,23 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -828,10 +819,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,7 +842,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -867,7 +858,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -875,127 +866,111 @@
         <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>138</v>
+        <v>122</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>138</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D7" s="4" t="s">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="D8" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="4">
         <v>1</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="2" t="s">
+      <c r="G8" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F9" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>108</v>
-      </c>
       <c r="F10" s="4">
-        <v>1</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="F11" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="F12" s="4">
         <v>3</v>
       </c>
     </row>
@@ -1015,13 +990,13 @@
           <x14:formula1>
             <xm:f>Option!$B$2:$B$93</xm:f>
           </x14:formula1>
-          <xm:sqref>D10:D12</xm:sqref>
+          <xm:sqref>D8:D10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Option!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E10:E12</xm:sqref>
+          <xm:sqref>E8:E10</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1048,7 +1023,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1064,22 +1039,22 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1119,10 +1094,10 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1130,10 +1105,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1141,460 +1116,460 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>